<commit_message>
Feat: update team and name
</commit_message>
<xml_diff>
--- a/data/purchase/shuttlecock_purchase.xlsx
+++ b/data/purchase/shuttlecock_purchase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\badminton-payment\shulttlecock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\badminton-payment\data\purchase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9422E6E-460E-4D70-A5EE-158B6132BB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE055122-1569-4A41-8073-DD89C2BE77A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -913,18 +913,19 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="6" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1008,15 +1009,15 @@
         <v>100</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G30" si="0">D3*E3+F3</f>
+        <f t="shared" ref="G3:G13" si="0">D3*E3+F3</f>
         <v>1490</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H30" si="1">E3*12</f>
+        <f t="shared" ref="H3:H13" si="1">E3*12</f>
         <v>24</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I30" si="2">ROUNDUP(G3/H3,0)</f>
+        <f t="shared" ref="I3:I13" si="2">ROUNDUP(G3/H3,0)</f>
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update: purchase shuttlecock Bullet tour 76
</commit_message>
<xml_diff>
--- a/data/purchase/shuttlecock_purchase.xlsx
+++ b/data/purchase/shuttlecock_purchase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\badminton-payment\data\purchase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1dd2fc4bf918acb/Projects/badminton-payment/data/purchase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F5B431-DECF-41F3-B4F7-5A271F77A913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{B1F5B431-DECF-41F3-B4F7-5A271F77A913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC953966-FB99-AA42-BB7D-333827578CAC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shuttlecock_buy" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>index</t>
   </si>
@@ -69,6 +67,9 @@
   </si>
   <si>
     <t>lingmei 80</t>
+  </si>
+  <si>
+    <t>Bullet tournament 76</t>
   </si>
 </sst>
 </file>
@@ -910,25 +911,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" customWidth="1"/>
+    <col min="8" max="8" width="4.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -957,7 +958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -989,7 +990,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1021,7 +1022,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1053,7 +1054,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1085,7 +1086,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1117,7 +1118,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1149,7 +1150,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1181,7 +1182,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1213,7 +1214,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1245,7 +1246,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1277,7 +1278,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1309,7 +1310,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1341,7 +1342,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1361,16 +1362,48 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G14" si="3">D14*E14+F14</f>
+        <f t="shared" ref="G14:G15" si="3">D14*E14+F14</f>
         <v>3550</v>
       </c>
       <c r="H14">
-        <f t="shared" ref="H14" si="4">E14*12</f>
+        <f t="shared" ref="H14:H15" si="4">E14*12</f>
         <v>60</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="I14" si="5">ROUNDUP(G14/H14,0)</f>
+        <f t="shared" ref="I14:I15" si="5">ROUNDUP(G14/H14,0)</f>
         <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45341</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <v>670</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>100</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>2780</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="5"/>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: buy shuttlecock 20240319
</commit_message>
<xml_diff>
--- a/data/purchase/shuttlecock_purchase.xlsx
+++ b/data/purchase/shuttlecock_purchase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1dd2fc4bf918acb/Projects/badminton-payment/data/purchase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{B1F5B431-DECF-41F3-B4F7-5A271F77A913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC953966-FB99-AA42-BB7D-333827578CAC}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{B1F5B431-DECF-41F3-B4F7-5A271F77A913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EDA8ADA-4AA0-4583-8990-931A28702D0A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shuttlecock_buy" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>index</t>
   </si>
@@ -614,10 +614,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -655,7 +659,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -761,7 +765,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -903,7 +907,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -911,25 +915,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" customWidth="1"/>
-    <col min="8" max="8" width="4.83203125" customWidth="1"/>
-    <col min="9" max="9" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -958,7 +962,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -990,7 +994,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1022,7 +1026,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1054,7 +1058,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1086,7 +1090,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1118,7 +1122,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1150,7 +1154,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1182,7 +1186,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1214,7 +1218,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1246,7 +1250,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1278,7 +1282,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1310,7 +1314,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1342,7 +1346,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1362,19 +1366,19 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G14:G15" si="3">D14*E14+F14</f>
+        <f t="shared" ref="G14:G16" si="3">D14*E14+F14</f>
         <v>3550</v>
       </c>
       <c r="H14">
-        <f t="shared" ref="H14:H15" si="4">E14*12</f>
+        <f t="shared" ref="H14:H16" si="4">E14*12</f>
         <v>60</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="I14:I15" si="5">ROUNDUP(G14/H14,0)</f>
+        <f t="shared" ref="I14:I16" si="5">ROUNDUP(G14/H14,0)</f>
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1402,6 +1406,38 @@
         <v>48</v>
       </c>
       <c r="I15">
+        <f t="shared" si="5"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45370</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>670</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>99</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>3449</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="5"/>
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Feat: support new folder format
</commit_message>
<xml_diff>
--- a/data/purchase/shuttlecock_purchase.xlsx
+++ b/data/purchase/shuttlecock_purchase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1dd2fc4bf918acb/Projects/badminton-payment/data/purchase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\badminton-payment\data\purchase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{B1F5B431-DECF-41F3-B4F7-5A271F77A913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EDA8ADA-4AA0-4583-8990-931A28702D0A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4CEFE2-9DCB-43B8-BE0A-84333A7619D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6135" yWindow="75" windowWidth="19515" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shuttlecock_buy" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>index</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Bullet tournament 76</t>
+  </si>
+  <si>
+    <t>RSL Gold</t>
   </si>
 </sst>
 </file>
@@ -612,10 +615,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -915,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,15 +1365,15 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G14:G16" si="3">D14*E14+F14</f>
+        <f t="shared" ref="G14:G19" si="3">D14*E14+F14</f>
         <v>3550</v>
       </c>
       <c r="H14">
-        <f t="shared" ref="H14:H16" si="4">E14*12</f>
+        <f t="shared" ref="H14:H19" si="4">E14*12</f>
         <v>60</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="I14:I16" si="5">ROUNDUP(G14/H14,0)</f>
+        <f t="shared" ref="I14:I19" si="5">ROUNDUP(G14/H14,0)</f>
         <v>60</v>
       </c>
     </row>
@@ -1440,6 +1439,102 @@
       <c r="I16">
         <f t="shared" si="5"/>
         <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45528</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>600</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>3600</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="4"/>
+        <v>72</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45600</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18">
+        <v>600</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>1200</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45627</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19">
+        <v>600</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>1200</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="5"/>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: sync, split_day and update payment 20241223 - 20250210
</commit_message>
<xml_diff>
--- a/data/purchase/shuttlecock_purchase.xlsx
+++ b/data/purchase/shuttlecock_purchase.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\badminton-payment\data\purchase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4CEFE2-9DCB-43B8-BE0A-84333A7619D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E13267E-A7CD-48E5-ADD3-72C833FF95AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6135" yWindow="75" windowWidth="19515" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shuttlecock_buy" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>index</t>
   </si>
@@ -73,6 +74,9 @@
   </si>
   <si>
     <t>RSL Gold</t>
+  </si>
+  <si>
+    <t>Yonex AS-10</t>
   </si>
 </sst>
 </file>
@@ -914,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G14:G19" si="3">D14*E14+F14</f>
+        <f t="shared" ref="G14:G20" si="3">D14*E14+F14</f>
         <v>3550</v>
       </c>
       <c r="H14">
@@ -1535,6 +1539,85 @@
       <c r="I19">
         <f t="shared" si="5"/>
         <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45658</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>810</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>8100</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20" si="6">E20*12</f>
+        <v>120</v>
+      </c>
+      <c r="I20">
+        <f t="shared" ref="I20" si="7">ROUNDUP(G20/H20,0)</f>
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A27C2286-E88C-46CC-BC19-F5D9EFC4153F}">
+  <dimension ref="A2:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45670</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>825</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2" si="0">D2*E2+F2</f>
+        <v>8250</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2" si="1">E2*12</f>
+        <v>120</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2" si="2">ROUNDUP(G2/H2,0)</f>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ีupdate: june - oct 2025
</commit_message>
<xml_diff>
--- a/data/purchase/shuttlecock_purchase.xlsx
+++ b/data/purchase/shuttlecock_purchase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\badminton-payment\data\purchase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E13267E-A7CD-48E5-ADD3-72C833FF95AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D5F0CC-D252-4C62-88B3-0B0D4D243FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>index</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Yonex AS-10</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -918,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,7 +1372,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G14:G20" si="3">D14*E14+F14</f>
+        <f t="shared" ref="G14:G21" si="3">D14*E14+F14</f>
         <v>3550</v>
       </c>
       <c r="H14">
@@ -1565,12 +1568,44 @@
         <v>8100</v>
       </c>
       <c r="H20">
-        <f t="shared" ref="H20" si="6">E20*12</f>
+        <f t="shared" ref="H20:H21" si="6">E20*12</f>
         <v>120</v>
       </c>
       <c r="I20">
-        <f t="shared" ref="I20" si="7">ROUNDUP(G20/H20,0)</f>
+        <f t="shared" ref="I20:I21" si="7">ROUNDUP(G20/H20,0)</f>
         <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45962</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21">
+        <v>720</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>1440</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="7"/>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>